<commit_message>
zipstream and dotenv is installed
</commit_message>
<xml_diff>
--- a/upload_templates/Catalogs_template.xlsx
+++ b/upload_templates/Catalogs_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\COA_pdf_generator\upload_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78D30AD7-0FA1-49CC-A180-FABD4B13AA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C400514F-DD10-4B63-9C92-58CB139E7792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD59E161-BE89-47A9-B50D-E69F46C75F8C}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>templateCode</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>formulation</t>
-  </si>
-  <si>
-    <t>molFormula</t>
   </si>
   <si>
     <t>observedMolMass</t>
@@ -905,13 +902,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE306C3-C282-4A35-B0FD-6F91CFB94D3D}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -953,9 +952,6 @@
       </c>
       <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>